<commit_message>
Adde VCO UI board outputs.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marten\Code\VCO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6BD65C-35AE-4C3C-89BA-209F82E5ECF5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82643DA3-B1D6-4783-B489-CE30AA2CE8DD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25545" windowHeight="18120" xr2:uid="{D120D5B5-606E-49B3-8DBD-703CF8BB7901}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="156">
   <si>
     <t>Comment</t>
   </si>
@@ -394,6 +394,105 @@
   </si>
   <si>
     <t>SGD</t>
+  </si>
+  <si>
+    <t>Potentiometer Alpha Taiwan C100K</t>
+  </si>
+  <si>
+    <t>Vertical PCB Mount 9mm 100k Potentiometer</t>
+  </si>
+  <si>
+    <t>AUXA1, AUXB1, FM2, PHASE2, PWM2, TUNE1</t>
+  </si>
+  <si>
+    <t>Resistor foo</t>
+  </si>
+  <si>
+    <t>CMP-v7h8zal8rowsx2pq2wqv-3</t>
+  </si>
+  <si>
+    <t>Multicomp MC0805B104K500A2.54MM</t>
+  </si>
+  <si>
+    <t>C1, C2, C3</t>
+  </si>
+  <si>
+    <t>WQP-PJ398SM</t>
+  </si>
+  <si>
+    <t>3.5mm Mono Jack PCB Mount</t>
+  </si>
+  <si>
+    <t>CV1, FM1, OUTA1, OUTB1, PHASE1, PWM1, SYNC1, TRIG1</t>
+  </si>
+  <si>
+    <t>PCB-msapmydrilbsl74io7e2-1</t>
+  </si>
+  <si>
+    <t>CMP-4jg5qs8nbosmqasq0ji9-3</t>
+  </si>
+  <si>
+    <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D11, D12, D13, D14, D15, D16</t>
+  </si>
+  <si>
+    <t>P1, P2</t>
+  </si>
+  <si>
+    <t>R1, R4</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>470</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20</t>
+  </si>
+  <si>
+    <t>Toggle Switch Momentary NO C NO</t>
+  </si>
+  <si>
+    <t>Momentary toggle switch</t>
+  </si>
+  <si>
+    <t>TS1, TS2</t>
+  </si>
+  <si>
+    <t>PCB-vhrr5z6azygjzs3qzahn-1</t>
+  </si>
+  <si>
+    <t>CMP-q68f8ms59qn9cyn6c5ql-1</t>
+  </si>
+  <si>
+    <t>SYM-168fdf857ed2c948-5</t>
+  </si>
+  <si>
+    <t>Schematic modified for easy side-by-side placement.</t>
+  </si>
+  <si>
+    <t>U1, U2</t>
+  </si>
+  <si>
+    <t>PCB-cyfl3a2g1l13gllfl41p-1</t>
+  </si>
+  <si>
+    <t>CMP-13951118-25</t>
+  </si>
+  <si>
+    <t>Bestep knob</t>
+  </si>
+  <si>
+    <t>Potentiometer know, plastic</t>
+  </si>
+  <si>
+    <t>see above</t>
   </si>
 </sst>
 </file>
@@ -440,7 +539,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -476,12 +575,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -493,6 +607,13 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -808,10 +929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91B5EE9-B2ED-4BDE-8F18-7EEE0F5A4ED1}">
-  <dimension ref="B3:I34"/>
+  <dimension ref="B3:I48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,7 +1022,7 @@
         <v>0.36299999999999999</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" ref="I5:I33" si="0">H5*G5</f>
+        <f t="shared" ref="I5:I47" si="0">H5*G5</f>
         <v>0.72599999999999998</v>
       </c>
     </row>
@@ -1653,22 +1774,396 @@
         <v>0.42199999999999999</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
+    <row r="34" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="G34" s="6">
+        <v>6</v>
+      </c>
+      <c r="H34" s="7">
+        <f>1.358*20.37/30</f>
+        <v>0.92208200000000007</v>
+      </c>
+      <c r="I34" s="7">
+        <f t="shared" si="0"/>
+        <v>5.5324920000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="3">
+        <v>6</v>
+      </c>
+      <c r="H35" s="4">
+        <f>1.358*3.89/30</f>
+        <v>0.17608733333333335</v>
+      </c>
+      <c r="I35" s="4">
+        <f t="shared" ref="I35" si="1">H35*G35</f>
+        <v>1.056524</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" s="3">
+        <v>3</v>
+      </c>
+      <c r="H36" s="4">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="I36" s="4">
+        <f t="shared" si="0"/>
+        <v>0.126</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="42" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G37" s="3">
+        <v>8</v>
+      </c>
+      <c r="H37" s="4">
+        <f>1.583*32/100</f>
+        <v>0.50656000000000001</v>
+      </c>
+      <c r="I37" s="4">
+        <f t="shared" si="0"/>
+        <v>4.0524800000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" ht="52.5" x14ac:dyDescent="0.25">
+      <c r="B38" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G38" s="3">
+        <v>16</v>
+      </c>
+      <c r="H38" s="4">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="I38" s="4">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B39" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G39" s="3">
+        <v>2</v>
+      </c>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G40" s="3">
+        <v>2</v>
+      </c>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G41" s="3">
+        <v>2</v>
+      </c>
+      <c r="H41" s="4">
+        <v>3.9E-2</v>
+      </c>
+      <c r="I41" s="4">
+        <f t="shared" si="0"/>
+        <v>7.8E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G42" s="3">
+        <v>1</v>
+      </c>
+      <c r="H42" s="4">
+        <v>3.9E-2</v>
+      </c>
+      <c r="I42" s="4">
+        <f t="shared" si="0"/>
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G43" s="3">
+        <v>1</v>
+      </c>
+      <c r="H43" s="4">
+        <v>3.9E-2</v>
+      </c>
+      <c r="I43" s="4">
+        <f t="shared" si="0"/>
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" ht="52.5" x14ac:dyDescent="0.25">
+      <c r="B44" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G44" s="3">
+        <v>16</v>
+      </c>
+      <c r="H44" s="4">
+        <v>3.9E-2</v>
+      </c>
+      <c r="I44" s="4">
+        <f t="shared" si="0"/>
+        <v>0.624</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G45" s="3">
+        <v>1</v>
+      </c>
+      <c r="H45" s="4">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="I45" s="4">
+        <f t="shared" si="0"/>
+        <v>0.17299999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="B46" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G46" s="3">
+        <v>2</v>
+      </c>
+      <c r="H46" s="4">
+        <f>1.358*6.5/10</f>
+        <v>0.88270000000000004</v>
+      </c>
+      <c r="I46" s="4">
+        <f t="shared" si="0"/>
+        <v>1.7654000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G47" s="3">
+        <v>2</v>
+      </c>
+      <c r="H47" s="4">
+        <v>0.74</v>
+      </c>
+      <c r="I47" s="4">
+        <f t="shared" si="0"/>
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="3">
-        <f>SUM(G4:G33)</f>
-        <v>92</v>
-      </c>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4">
-        <f>SUM(I4:I33)</f>
-        <v>16.121000000000002</v>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="3">
+        <f>SUM(G4:G47)</f>
+        <v>160</v>
+      </c>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4">
+        <f>SUM(I4:I47)</f>
+        <v>32.286895999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>